<commit_message>
modified function. added some comments. updated charts accordingly
</commit_message>
<xml_diff>
--- a/wl_rf_analysis/feature_results.xlsx
+++ b/wl_rf_analysis/feature_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1321e406685d2c32/rpi/20fall/ITWS-4350/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="11_F25DC773A252ABDACC1048E471DE48805ADE58E7" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ACC97DAD-611B-4566-B141-AECE2D58F845}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="11_F25DC773A252ABDACC1048E471DE48805ADE58E7" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FE140C1-1A82-4C4C-B16B-6B54E773EF56}"/>
   <bookViews>
-    <workbookView xWindow="7908" yWindow="4524" windowWidth="11352" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11616" yWindow="1548" windowWidth="18816" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="214" zoomScaleNormal="214" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,16 +411,16 @@
         <v>20</v>
       </c>
       <c r="D2">
-        <v>0.77800000000000002</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="E2">
-        <v>6.88E-2</v>
+        <v>6.54E-2</v>
       </c>
       <c r="F2">
-        <v>0.20200000000000001</v>
+        <v>0.21</v>
       </c>
       <c r="G2">
-        <v>6.93E-2</v>
+        <v>6.4600000000000005E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -434,16 +434,16 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>0.36099999999999999</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="E3">
-        <v>1.03E-2</v>
+        <v>9.6100000000000005E-3</v>
       </c>
       <c r="F3">
-        <v>0.35899999999999999</v>
+        <v>0.372</v>
       </c>
       <c r="G3">
-        <v>3.04E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -457,16 +457,16 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>0.127</v>
+        <v>0.111</v>
       </c>
       <c r="E4">
-        <v>3.4499999999999999E-3</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="F4">
-        <v>0.64200000000000002</v>
+        <v>0.65900000000000003</v>
       </c>
       <c r="G4">
-        <v>6.7400000000000003E-3</v>
+        <v>6.1199999999999996E-3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -480,16 +480,16 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>8.4500000000000006E-2</v>
+        <v>7.2400000000000006E-2</v>
       </c>
       <c r="E5">
-        <v>2.6800000000000001E-3</v>
+        <v>2.48E-3</v>
       </c>
       <c r="F5">
-        <v>0.86599999999999999</v>
+        <v>0.88400000000000001</v>
       </c>
       <c r="G5">
-        <v>4.5599999999999998E-3</v>
+        <v>4.13E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -503,16 +503,16 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>2.98E-2</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="E6">
-        <v>6.4099999999999997E-4</v>
+        <v>5.8699999999999996E-4</v>
       </c>
       <c r="F6">
-        <v>0.88700000000000001</v>
+        <v>0.86799999999999999</v>
       </c>
       <c r="G6">
-        <v>1.47E-3</v>
+        <v>1.31E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -526,16 +526,16 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>2.1700000000000001E-2</v>
+        <v>1.78E-2</v>
       </c>
       <c r="E7">
-        <v>3.8699999999999997E-4</v>
+        <v>3.5300000000000002E-4</v>
       </c>
       <c r="F7">
-        <v>0.78300000000000003</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="G7">
-        <v>9.7300000000000002E-4</v>
+        <v>8.6799999999999996E-4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -549,16 +549,16 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>1.54E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="E8">
-        <v>2.24E-4</v>
+        <v>2.04E-4</v>
       </c>
       <c r="F8">
-        <v>0.68200000000000005</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="G8">
-        <v>6.2799999999999998E-4</v>
+        <v>5.5900000000000004E-4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -571,17 +571,17 @@
       <c r="C9">
         <v>5</v>
       </c>
-      <c r="D9">
-        <v>1.0499999999999999E-3</v>
+      <c r="D9" s="1">
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E9" s="1">
-        <v>2.6699999999999998E-5</v>
+        <v>2.4000000000000001E-5</v>
       </c>
       <c r="F9">
-        <v>0.44</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="G9">
-        <v>1.9900000000000001E-4</v>
+        <v>1.75E-4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -595,16 +595,16 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <v>3.6900000000000002E-4</v>
+        <v>2.7599999999999999E-4</v>
       </c>
       <c r="E10" s="1">
-        <v>9.1400000000000006E-6</v>
+        <v>8.1499999999999999E-6</v>
       </c>
       <c r="F10">
-        <v>0.32700000000000001</v>
+        <v>0.316</v>
       </c>
       <c r="G10" s="1">
-        <v>9.7200000000000004E-5</v>
+        <v>8.53E-5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -618,16 +618,16 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <v>1.8699999999999999E-4</v>
+        <v>1.3799999999999999E-4</v>
       </c>
       <c r="E11" s="1">
-        <v>2.0000000000000002E-5</v>
+        <v>1.8E-5</v>
       </c>
       <c r="F11">
-        <v>0.307</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="G11" s="1">
-        <v>7.3499999999999998E-5</v>
+        <v>6.4399999999999993E-5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -641,16 +641,16 @@
         <v>4</v>
       </c>
       <c r="D12">
-        <v>2.7799999999999998E-4</v>
+        <v>2.0699999999999999E-4</v>
       </c>
       <c r="E12" s="1">
-        <v>1.22E-5</v>
+        <v>1.1E-5</v>
       </c>
       <c r="F12">
-        <v>0.28799999999999998</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="G12" s="1">
-        <v>6.9400000000000006E-5</v>
+        <v>6.0800000000000001E-5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -664,16 +664,16 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <v>1.47E-4</v>
+        <v>1.08E-4</v>
       </c>
       <c r="E13" s="1">
-        <v>6.6899999999999997E-7</v>
+        <v>5.8999999999999996E-7</v>
       </c>
       <c r="F13">
-        <v>0.13900000000000001</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="G13" s="1">
-        <v>1.7499999999999998E-5</v>
+        <v>1.5299999999999999E-5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -687,16 +687,16 @@
         <v>3</v>
       </c>
       <c r="D14" s="1">
-        <v>4.9700000000000002E-5</v>
+        <v>3.5800000000000003E-5</v>
       </c>
       <c r="E14" s="1">
-        <v>2.3099999999999999E-7</v>
+        <v>2.03E-7</v>
       </c>
       <c r="F14">
-        <v>0.151</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="G14" s="1">
-        <v>1.5400000000000002E-5</v>
+        <v>1.34E-5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -710,16 +710,16 @@
         <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>1.8199999999999999E-5</v>
+        <v>1.29E-5</v>
       </c>
       <c r="E15" s="1">
-        <v>9.1100000000000002E-8</v>
+        <v>8.0000000000000002E-8</v>
       </c>
       <c r="F15">
-        <v>6.5500000000000003E-2</v>
+        <v>6.2300000000000001E-2</v>
       </c>
       <c r="G15" s="1">
-        <v>1.19E-5</v>
+        <v>1.04E-5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -733,16 +733,62 @@
         <v>2</v>
       </c>
       <c r="D16" s="1">
-        <v>8.7399999999999993E-6</v>
+        <v>6.1199999999999999E-6</v>
       </c>
       <c r="E16" s="1">
-        <v>1.6099999999999999E-8</v>
+        <v>1.4100000000000001E-8</v>
       </c>
       <c r="F16">
-        <v>4.9599999999999998E-2</v>
+        <v>4.7199999999999999E-2</v>
       </c>
       <c r="G16" s="1">
-        <v>8.5599999999999994E-6</v>
+        <v>7.5000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4.3599999999999998E-6</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.4699999999999999E-8</v>
+      </c>
+      <c r="F17">
+        <v>3.6700000000000003E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1.03E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.6500000000000001E-6</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4.3800000000000002E-9</v>
+      </c>
+      <c r="F18">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>8.1100000000000003E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wrapping up. added a few visualization and tests
</commit_message>
<xml_diff>
--- a/wl_rf_analysis/feature_results.xlsx
+++ b/wl_rf_analysis/feature_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1321e406685d2c32/rpi/20fall/ITWS-4350/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="238" documentId="11_F25DC773A252ABDACC1048E471DE48805ADE58E7" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{331DAC24-2AF0-45E5-A450-0C5CC58FB0ED}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="11_F25DC773A252ABDACC1048E471DE48805ADE58E7" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ECE05ED3-9A3B-4F97-8594-7D38D74DB6B8}"/>
   <bookViews>
-    <workbookView xWindow="6252" yWindow="1572" windowWidth="18816" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9768" yWindow="1440" windowWidth="18648" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection sqref="A1:G18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,6 +792,29 @@
         <v>8.1100000000000003E-6</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7.92E-7</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3.8500000000000001E-10</v>
+      </c>
+      <c r="F19">
+        <v>6.4900000000000001E-3</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2.0200000000000001E-6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>